<commit_message>
GetMachines now also retrieves machine keys.
</commit_message>
<xml_diff>
--- a/Config/Machines.xlsx
+++ b/Config/Machines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\UiPath\OrchestratorManager\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C8AF14-54B1-4177-960C-63285B2D1240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA438D6-4B60-4417-ACD7-5424702EC69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Type</t>
   </si>
@@ -49,28 +49,7 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Standard1</t>
-  </si>
-  <si>
-    <t>Desc1</t>
-  </si>
-  <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>JPLPTMATEUS</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
-    <t>MATEUSCRUZ-PC</t>
-  </si>
-  <si>
-    <t>DESKTOP-696S8E5</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -115,12 +94,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,8 +145,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0">
-  <autoFilter ref="A1:D11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D101" totalsRowShown="0">
+  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
@@ -178,8 +158,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:B101" totalsRowShown="0">
+  <autoFilter ref="A1:B101" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Id" dataDxfId="1"/>
@@ -189,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E14">
-  <autoFilter ref="A1:E14" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E101">
+  <autoFilter ref="A1:E101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Type" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name"/>
@@ -467,9 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -494,15 +472,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -561,7 +531,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,16 +545,11 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>240725</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
@@ -612,10 +577,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,49 +605,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2">
-        <v>19835</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>21370</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>225775</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
@@ -726,10 +665,269 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E101" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Added the posibility to specify the machine key when creating a machine.
</commit_message>
<xml_diff>
--- a/Config/Machines.xlsx
+++ b/Config/Machines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA438D6-4B60-4417-ACD7-5424702EC69E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8DD5D8-74AF-41D9-B3B3-A9DCD456E4B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -579,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>